<commit_message>
correction donnees statstiques Economique
</commit_message>
<xml_diff>
--- a/Donnees/Statistiques Démographiques et sociales/Education/Tableaux Education_portail.xlsx
+++ b/Donnees/Statistiques Démographiques et sociales/Education/Tableaux Education_portail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\2025\Annuaire des Statistiques Socio-démographiques_Edition 2025_VP\Atelier de Finalisation et Validation de l'Annuaire 2025\Portail DSDSG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Ansade_Project\Donnees\Statistiques Démographiques et sociales\Education\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED78332-BDDF-454E-B352-0BE1228195D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783FB5C1-06A1-4A73-AAA8-EB77A5C09F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{1F576A4F-F94E-4D0F-B3FB-7D4F02E6ECAF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F576A4F-F94E-4D0F-B3FB-7D4F02E6ECAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>Wilaya</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Tableau : Evolution du taux d’analphabétisme selon la wilaya et le sexe durant la période 2000-2023</t>
+  </si>
+  <si>
+    <t>2023~Ensemble</t>
   </si>
 </sst>
 </file>
@@ -893,30 +896,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4302CBB-9F3E-4B35-A39F-FEB9F6FF3862}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" style="8" customWidth="1"/>
     <col min="9" max="9" width="14" style="8" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -939,16 +942,16 @@
         <v>53</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -980,7 +983,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>46.9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1172,7 +1175,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1364,7 +1367,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>47</v>
       </c>
@@ -1492,15 +1495,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>69</v>
       </c>
@@ -1509,7 +1512,7 @@
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
     </row>
-    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="32"/>
       <c r="B2" s="19" t="s">
         <v>63</v>
@@ -1521,7 +1524,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>54</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>56</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>59</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>62</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>47</v>
       </c>
@@ -1669,18 +1672,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C0C857-13F2-44B9-B9F3-59C98BEF28B6}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" customWidth="1"/>
-    <col min="2" max="9" width="10.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
         <v>68</v>
       </c>
@@ -1694,7 +1697,7 @@
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
     </row>
-    <row r="2" spans="1:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>40</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>83.2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
         <v>4</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>88.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>89.9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +1921,7 @@
         <v>102.9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>7</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>105.1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
         <v>8</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>129.9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>37</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>118.9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27" t="s">
         <v>10</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>114.5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>38</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>79.7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
         <v>11</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>122.1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>12</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>127.4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
         <v>39</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>106.3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27" t="s">
         <v>13</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>101.2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>15</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>108.5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
         <v>16</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>109.2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
         <v>47</v>
       </c>

</xml_diff>